<commit_message>
UPDATE : Update rencana dalam Use Cases/Tabel Kebutuhan.xlsx
</commit_message>
<xml_diff>
--- a/Use Cases/Tabel Kebutuhan.xlsx
+++ b/Use Cases/Tabel Kebutuhan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher Clement\OneDrive\Documents\Universitas - MatKul\BPKK (Framework Programming)\pbkk-fp-kel-6\Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A61DD41-BC23-4770-AC6E-1D82DEB77A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6BFD4E-85DB-4375-9BCF-DED8AB4E2807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8747CDE8-8086-4547-8632-5E839A464BBC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Kebutuhan Bisnis</t>
   </si>
@@ -118,13 +118,55 @@
   </si>
   <si>
     <t>Otomatis mengganti isi dalam kamus sesuai ajuan yang disetujui (mencatat ajuan yang mengubah)</t>
+  </si>
+  <si>
+    <t>Kelas View Baru</t>
+  </si>
+  <si>
+    <t>Kelas Controller Baru</t>
+  </si>
+  <si>
+    <t>Kelas Model Baru + Tabel Baru</t>
+  </si>
+  <si>
+    <t>Kelas lain Baru</t>
+  </si>
+  <si>
+    <t>2 Controller, viewer dan CRUD</t>
+  </si>
+  <si>
+    <t>Listener, update jumlah soal saat soal baru ditambah</t>
+  </si>
+  <si>
+    <t>2 View, Form tambah soal and viewer untuk pengerjaan soal</t>
+  </si>
+  <si>
+    <t>2 View, Form tambah paket and Viewer paket soal</t>
+  </si>
+  <si>
+    <t>1 Model (id, nama paket, deskripsi paket, jumlah soal) | 1 paket banyak soal</t>
+  </si>
+  <si>
+    <t>1 Model (id, id paket, tipe soal (pilihan 4 opsi/isian), soal, jawaban) | 1 soal 1 paket</t>
+  </si>
+  <si>
+    <t>2 Controller, 1 menampilkan dan mengecek jawaban dan CRUD untuk form</t>
+  </si>
+  <si>
+    <t>Event, jika soal ditambah</t>
+  </si>
+  <si>
+    <t>! Ide cache = Bantu export semua kata dalam suatu bahasa menjadi csv lalu buat link sementara. Simpan file dalam cache seandainya ada user lain yang download juga.</t>
+  </si>
+  <si>
+    <t>! Ide job &amp; queue = Bantu supaya kalau export gagal, otomatis dicoba lagi dan kalau lama, otomatis gk bikin site ngehang.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +177,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -214,12 +262,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -233,21 +299,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -564,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A24490D-006E-4D47-BD73-535319BBBF51}">
-  <dimension ref="C6:F27"/>
+  <dimension ref="C4:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C25"/>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,10 +654,20 @@
     <col min="4" max="4" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="7" max="10" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
@@ -592,187 +680,291 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="8" t="s">
+      <c r="G6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="3:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="8" t="s">
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="3:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="10"/>
-      <c r="D10" s="6"/>
+      <c r="G9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="3:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="10"/>
-      <c r="D11" s="5" t="s">
+    <row r="11" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="9"/>
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="3:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="10"/>
-      <c r="D12" s="5"/>
+      <c r="G11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="9"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="3:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="10"/>
-      <c r="D13" s="5"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="9"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C14" s="10"/>
-      <c r="D14" s="5" t="s">
+      <c r="G13" s="14"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C14" s="9"/>
+      <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C15" s="9"/>
-      <c r="D15" s="5"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C15" s="8"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="3:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="8" t="s">
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="3:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="10"/>
-      <c r="D17" s="5"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="9"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="3:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="10"/>
-      <c r="D18" s="5" t="s">
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="9"/>
+      <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="3:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="10"/>
-      <c r="D19" s="5"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="9"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="3:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="10"/>
-      <c r="D20" s="5"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="9"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C21" s="10"/>
-      <c r="D21" s="5" t="s">
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C21" s="9"/>
+      <c r="D21" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C22" s="10"/>
-      <c r="D22" s="5"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C22" s="9"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C23" s="10"/>
-      <c r="D23" s="5"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="3:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C23" s="9"/>
+      <c r="D23" s="6"/>
       <c r="E23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C24" s="10"/>
-      <c r="D24" s="5"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C24" s="9"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C25" s="9"/>
-      <c r="D25" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C25" s="8"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F25" s="5"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E27" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
     <mergeCell ref="D21:D25"/>
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="D16:D17"/>
@@ -784,6 +976,7 @@
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="D14:D15"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIX : Tambah header di form kata + Tambah notifikasi. FIX : Model Soal. FIX : Seeder, create user and bahasa
</commit_message>
<xml_diff>
--- a/Use Cases/Tabel Kebutuhan.xlsx
+++ b/Use Cases/Tabel Kebutuhan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher Clement\OneDrive\Documents\Universitas - MatKul\BPKK (Framework Programming)\pbkk-fp-kel-6\Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6BFD4E-85DB-4375-9BCF-DED8AB4E2807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369E328F-E30A-4A46-A246-94ADA2595E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8747CDE8-8086-4547-8632-5E839A464BBC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Kebutuhan Bisnis</t>
   </si>
@@ -132,41 +132,47 @@
     <t>Kelas lain Baru</t>
   </si>
   <si>
-    <t>2 Controller, viewer dan CRUD</t>
-  </si>
-  <si>
-    <t>Listener, update jumlah soal saat soal baru ditambah</t>
-  </si>
-  <si>
-    <t>2 View, Form tambah soal and viewer untuk pengerjaan soal</t>
-  </si>
-  <si>
     <t>2 View, Form tambah paket and Viewer paket soal</t>
   </si>
   <si>
     <t>1 Model (id, nama paket, deskripsi paket, jumlah soal) | 1 paket banyak soal</t>
   </si>
   <si>
-    <t>1 Model (id, id paket, tipe soal (pilihan 4 opsi/isian), soal, jawaban) | 1 soal 1 paket</t>
-  </si>
-  <si>
-    <t>2 Controller, 1 menampilkan dan mengecek jawaban dan CRUD untuk form</t>
-  </si>
-  <si>
-    <t>Event, jika soal ditambah</t>
-  </si>
-  <si>
     <t>! Ide cache = Bantu export semua kata dalam suatu bahasa menjadi csv lalu buat link sementara. Simpan file dalam cache seandainya ada user lain yang download juga.</t>
   </si>
   <si>
-    <t>! Ide job &amp; queue = Bantu supaya kalau export gagal, otomatis dicoba lagi dan kalau lama, otomatis gk bikin site ngehang.</t>
+    <t>1 controller, CRUD</t>
+  </si>
+  <si>
+    <t>1 untuk soal :  (id, id paket, tipe soal (pilihan 4 opsi/isian), soal, jawaban) | 1 soal 1 paket</t>
+  </si>
+  <si>
+    <t>2 Controller, CRUD + Mengolah jawaban (Cek + Simpan di cache sampai user pergi)</t>
+  </si>
+  <si>
+    <t>Event, jika user session expired. Listener, discard hasil pengerjaan user di cache.</t>
+  </si>
+  <si>
+    <t>1 Model</t>
+  </si>
+  <si>
+    <t>3 View, Form tambah + edit soal, viewer untuk pengerjaan soal, dan view hasil pengerjaan</t>
+  </si>
+  <si>
+    <t>! Ide Factory = Untuk paket + soal. Supaya relasinya otomatis terbentuk</t>
+  </si>
+  <si>
+    <t>! Ide job &amp; queue = Bantu supaya kalau export gagal, otomatis dicoba lagi dan kalau lama, otomatis gk bikin site ngehang.  || Job : Weekly defrag database?</t>
+  </si>
+  <si>
+    <t>|| Job, Queue, dan broadcast : Export soal sebagai pdf?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +189,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -300,6 +314,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -315,18 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -642,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A24490D-006E-4D47-BD73-535319BBBF51}">
-  <dimension ref="C4:J27"/>
+  <dimension ref="C2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11:I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,14 +672,24 @@
     <col min="7" max="10" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C2" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -680,278 +705,278 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="12" t="s">
+      <c r="I9" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="9"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="G11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="12" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="9"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="3:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="9"/>
-      <c r="D13" s="6"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C14" s="9"/>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C15" s="8"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="9"/>
-      <c r="D17" s="6"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="9"/>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="13"/>
+      <c r="D18" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="9"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" spans="3:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="9"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
     </row>
     <row r="21" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C21" s="9"/>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="10" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
     <row r="22" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C22" s="9"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
     </row>
     <row r="23" spans="3:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C23" s="9"/>
-      <c r="D23" s="6"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
     </row>
     <row r="24" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C24" s="9"/>
-      <c r="D24" s="6"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C25" s="8"/>
-      <c r="D25" s="6"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F25" s="5"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E26" s="1"/>
@@ -960,14 +985,7 @@
       <c r="E27" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="D16:D17"/>
+  <mergeCells count="13">
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C9:C15"/>
@@ -975,6 +993,12 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="D14:D15"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="D16:D17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>